<commit_message>
- added seeder for Slots - updated spreadsheet with slots
</commit_message>
<xml_diff>
--- a/server/database/seeds/seeds.xlsx
+++ b/server/database/seeds/seeds.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B4BEC-7B81-445E-ADD0-D15668079E4D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5D46B7-FF77-4C64-815F-2E8D811AC78A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guns" sheetId="1" r:id="rId1"/>
+    <sheet name="Slots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -59,6 +60,54 @@
   </si>
   <si>
     <t>7.62x39</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>Bipod</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Dust Cover</t>
+  </si>
+  <si>
+    <t>Gas Mod</t>
+  </si>
+  <si>
+    <t>Handguard</t>
+  </si>
+  <si>
+    <t>Magazine</t>
+  </si>
+  <si>
+    <t>Mount</t>
+  </si>
+  <si>
+    <t>Muzzle</t>
+  </si>
+  <si>
+    <t>Optic</t>
+  </si>
+  <si>
+    <t>Pistol Grip</t>
+  </si>
+  <si>
+    <t>Receiver</t>
+  </si>
+  <si>
+    <t>Sight</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Tactical Grip</t>
+  </si>
+  <si>
+    <t>Tactical Mod</t>
   </si>
 </sst>
 </file>
@@ -387,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,4 +534,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C680656-C6FA-474A-ADDB-003C079833C1}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added seeder for attachments - includes seeding of the relationship to a slot Replaced horizontal/vertical recoil modifier fields with recoil_modifier
</commit_message>
<xml_diff>
--- a/server/database/seeds/seeds.xlsx
+++ b/server/database/seeds/seeds.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B68D96-F411-4A15-85C8-353915287749}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3399A732-B71C-4174-8674-AC461B223AC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guns" sheetId="1" r:id="rId1"/>
@@ -2579,7 +2579,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="188">
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2587,173 +2587,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2931,1493 +2764,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4719,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -6432,61 +4778,61 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H65">
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Assault rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Assault carbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Submachine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Shotgun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Designated marksman rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6603,8 +4949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ED6926-697D-47E2-A2FD-3B0DE769BE34}">
   <dimension ref="A1:D718"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16670,7 +15016,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="187" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated seed file with Gunslot data
</commit_message>
<xml_diff>
--- a/server/database/seeds/seeds.xlsx
+++ b/server/database/seeds/seeds.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3399A732-B71C-4174-8674-AC461B223AC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60D508-0FFC-49AE-95F5-6D22C8581827}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guns" sheetId="1" r:id="rId1"/>
     <sheet name="Slots" sheetId="2" r:id="rId2"/>
     <sheet name="Attachments" sheetId="3" r:id="rId3"/>
+    <sheet name="Gunslot" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="840">
   <si>
     <t>name</t>
   </si>
@@ -2512,6 +2513,36 @@
   </si>
   <si>
     <t>PM (t) pistol</t>
+  </si>
+  <si>
+    <t>gun</t>
+  </si>
+  <si>
+    <t>Rear sight</t>
+  </si>
+  <si>
+    <t>Gas block</t>
+  </si>
+  <si>
+    <t>Charge handle</t>
+  </si>
+  <si>
+    <t>Pistol grip</t>
+  </si>
+  <si>
+    <t>Launcher</t>
+  </si>
+  <si>
+    <t>Front sight</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Tactical</t>
+  </si>
+  <si>
+    <t>Foregrip</t>
   </si>
 </sst>
 </file>
@@ -2592,11 +2623,158 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9999FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="9" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2622,158 +2800,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="9" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9999FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4778,62 +4809,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H65">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"Assault rifle"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
-      <formula>"Assault carbine"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
-      <formula>"Submachine gun"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"Shotgun"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
-      <formula>"Designated marksman rifle"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"Sniper rifle"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Pistol"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>603</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>603</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>603</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"Pistol"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+      <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+      <formula>"Designated marksman rifle"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>"Shotgun"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+      <formula>"Submachine gun"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="17" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"Light machine gun"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="18" operator="equal">
+      <formula>"Assault carbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>603</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Light machine gun"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Sniper rifle"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+      <formula>"Assault rifle"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4949,7 +4980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ED6926-697D-47E2-A2FD-3B0DE769BE34}">
   <dimension ref="A1:D718"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -15021,4 +15052,3297 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB657F5-FC13-4A6B-958C-A0D5C6E6E70D}">
+  <dimension ref="A1:B409"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added seeder for GunSlot, and: - added incrementing id field to gun_slot table - fixed mistake in seeds file (unrecognised slot in GunSlots 'Tactical')
</commit_message>
<xml_diff>
--- a/server/database/seeds/seeds.xlsx
+++ b/server/database/seeds/seeds.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60D508-0FFC-49AE-95F5-6D22C8581827}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970B931B-7E74-4251-BAC8-11131DFC74FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guns" sheetId="1" r:id="rId1"/>
     <sheet name="Slots" sheetId="2" r:id="rId2"/>
     <sheet name="Attachments" sheetId="3" r:id="rId3"/>
-    <sheet name="Gunslot" sheetId="4" r:id="rId4"/>
+    <sheet name="GunSlots" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="831">
   <si>
     <t>name</t>
   </si>
@@ -2516,33 +2516,6 @@
   </si>
   <si>
     <t>gun</t>
-  </si>
-  <si>
-    <t>Rear sight</t>
-  </si>
-  <si>
-    <t>Gas block</t>
-  </si>
-  <si>
-    <t>Charge handle</t>
-  </si>
-  <si>
-    <t>Pistol grip</t>
-  </si>
-  <si>
-    <t>Launcher</t>
-  </si>
-  <si>
-    <t>Front sight</t>
-  </si>
-  <si>
-    <t>Scope</t>
-  </si>
-  <si>
-    <t>Tactical</t>
-  </si>
-  <si>
-    <t>Foregrip</t>
   </si>
 </sst>
 </file>
@@ -4980,8 +4953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ED6926-697D-47E2-A2FD-3B0DE769BE34}">
   <dimension ref="A1:D718"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A589" workbookViewId="0">
+      <selection activeCell="B413" sqref="B413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15056,10 +15029,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB657F5-FC13-4A6B-958C-A0D5C6E6E70D}">
-  <dimension ref="A1:B409"/>
+  <dimension ref="A1:B396"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="P252" sqref="P252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15082,7 +15055,7 @@
         <v>768</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>832</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -15090,7 +15063,7 @@
         <v>768</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>835</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -15098,7 +15071,7 @@
         <v>768</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -15106,7 +15079,7 @@
         <v>768</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>834</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -15114,7 +15087,7 @@
         <v>768</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -15122,7 +15095,7 @@
         <v>768</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -15130,7 +15103,7 @@
         <v>768</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -15138,7 +15111,7 @@
         <v>768</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -15146,15 +15119,15 @@
         <v>768</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>833</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>836</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -15162,7 +15135,7 @@
         <v>755</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>832</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -15170,7 +15143,7 @@
         <v>755</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>835</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -15178,7 +15151,7 @@
         <v>755</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -15186,7 +15159,7 @@
         <v>755</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -15194,7 +15167,7 @@
         <v>755</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -15202,7 +15175,7 @@
         <v>755</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>831</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -15210,7 +15183,7 @@
         <v>755</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -15218,23 +15191,23 @@
         <v>755</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>833</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>836</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -15242,7 +15215,7 @@
         <v>749</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -15250,7 +15223,7 @@
         <v>749</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -15258,7 +15231,7 @@
         <v>749</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -15266,7 +15239,7 @@
         <v>749</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -15274,23 +15247,23 @@
         <v>749</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>749</v>
+        <v>767</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>749</v>
+        <v>767</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -15298,7 +15271,7 @@
         <v>767</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -15306,7 +15279,7 @@
         <v>767</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -15314,23 +15287,23 @@
         <v>767</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>833</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -15338,7 +15311,7 @@
         <v>760</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -15346,7 +15319,7 @@
         <v>760</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -15354,23 +15327,23 @@
         <v>760</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>833</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -15378,7 +15351,7 @@
         <v>758</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -15386,7 +15359,7 @@
         <v>758</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>834</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -15394,7 +15367,7 @@
         <v>758</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>831</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -15402,23 +15375,23 @@
         <v>758</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>837</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -15426,7 +15399,7 @@
         <v>753</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -15434,7 +15407,7 @@
         <v>753</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -15442,7 +15415,7 @@
         <v>753</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -15450,7 +15423,7 @@
         <v>753</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -15458,7 +15431,7 @@
         <v>753</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -15466,23 +15439,23 @@
         <v>753</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -15490,7 +15463,7 @@
         <v>764</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -15498,7 +15471,7 @@
         <v>764</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -15506,7 +15479,7 @@
         <v>764</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -15514,7 +15487,7 @@
         <v>764</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -15522,7 +15495,7 @@
         <v>764</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -15530,23 +15503,23 @@
         <v>764</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>764</v>
+        <v>744</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>764</v>
+        <v>744</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -15554,7 +15527,7 @@
         <v>744</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -15562,7 +15535,7 @@
         <v>744</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -15570,7 +15543,7 @@
         <v>744</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -15578,7 +15551,7 @@
         <v>744</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -15586,23 +15559,23 @@
         <v>744</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>744</v>
+        <v>769</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>744</v>
+        <v>769</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -15610,7 +15583,7 @@
         <v>769</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -15618,7 +15591,7 @@
         <v>769</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>835</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -15626,7 +15599,7 @@
         <v>769</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -15634,7 +15607,7 @@
         <v>769</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -15642,7 +15615,7 @@
         <v>769</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -15650,7 +15623,7 @@
         <v>769</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -15658,31 +15631,31 @@
         <v>769</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>769</v>
+        <v>737</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>769</v>
+        <v>737</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>769</v>
+        <v>737</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>833</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -15690,7 +15663,7 @@
         <v>737</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>832</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -15698,7 +15671,7 @@
         <v>737</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>835</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -15706,7 +15679,7 @@
         <v>737</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -15714,7 +15687,7 @@
         <v>737</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>834</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -15722,39 +15695,39 @@
         <v>737</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>737</v>
+        <v>761</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>831</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>737</v>
+        <v>761</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>737</v>
+        <v>761</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>737</v>
+        <v>761</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>833</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -15762,7 +15735,7 @@
         <v>761</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>832</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -15770,7 +15743,7 @@
         <v>761</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>835</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -15778,7 +15751,7 @@
         <v>761</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -15786,7 +15759,7 @@
         <v>761</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>834</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -15794,7 +15767,7 @@
         <v>761</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -15802,47 +15775,47 @@
         <v>761</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>836</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>833</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -15850,7 +15823,7 @@
         <v>762</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>832</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -15858,7 +15831,7 @@
         <v>762</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>835</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -15866,7 +15839,7 @@
         <v>762</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -15874,55 +15847,55 @@
         <v>762</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>834</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>831</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>836</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>833</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -15930,7 +15903,7 @@
         <v>746</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>832</v>
+        <v>23</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -15938,7 +15911,7 @@
         <v>746</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>835</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -15946,7 +15919,7 @@
         <v>746</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -15954,63 +15927,63 @@
         <v>746</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>834</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>831</v>
+        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>836</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>833</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -16018,7 +15991,7 @@
         <v>757</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>832</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -16026,52 +15999,52 @@
         <v>757</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>835</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>834</v>
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>831</v>
+        <v>21</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>836</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>23</v>
@@ -16079,7 +16052,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>16</v>
@@ -16087,10 +16060,10 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>833</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -16098,20 +16071,20 @@
         <v>743</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>832</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>835</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>18</v>
@@ -16119,15 +16092,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>834</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>21</v>
@@ -16135,15 +16108,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>831</v>
+        <v>22</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>23</v>
@@ -16151,7 +16124,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>16</v>
@@ -16159,7 +16132,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>17</v>
@@ -16167,895 +16140,895 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>833</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>832</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>835</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>834</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>835</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>831</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>831</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>766</v>
+        <v>741</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>766</v>
+        <v>741</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>832</v>
+        <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>835</v>
+        <v>21</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>752</v>
+        <v>9</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>752</v>
+        <v>9</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>752</v>
+        <v>9</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>833</v>
+        <v>20</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>832</v>
+        <v>21</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>741</v>
+        <v>9</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>741</v>
+        <v>8</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>741</v>
+        <v>8</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>741</v>
+        <v>8</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>833</v>
+        <v>23</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>832</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>835</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>834</v>
+        <v>21</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>9</v>
+        <v>770</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>9</v>
+        <v>774</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>9</v>
+        <v>774</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>833</v>
+        <v>22</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>8</v>
+        <v>774</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>8</v>
+        <v>774</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>833</v>
+        <v>23</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>770</v>
+        <v>96</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>832</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>770</v>
+        <v>96</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>831</v>
+        <v>18</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>831</v>
+        <v>17</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>96</v>
+        <v>775</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>96</v>
+        <v>775</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>831</v>
+        <v>21</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>96</v>
+        <v>775</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>96</v>
+        <v>775</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>96</v>
+        <v>775</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>833</v>
+        <v>23</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>834</v>
+        <v>12</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>833</v>
+        <v>16</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>832</v>
+        <v>17</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>781</v>
+        <v>789</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>781</v>
+        <v>789</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>834</v>
+        <v>16</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>781</v>
+        <v>789</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>831</v>
+        <v>14</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>833</v>
+        <v>21</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>834</v>
+        <v>23</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>16</v>
@@ -17063,63 +17036,63 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>834</v>
+        <v>19</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>834</v>
+        <v>21</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>832</v>
+        <v>12</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>18</v>
@@ -17127,167 +17100,167 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>837</v>
+        <v>24</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>833</v>
+        <v>19</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>834</v>
+        <v>18</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>833</v>
+        <v>16</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>831</v>
+        <v>19</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>836</v>
+        <v>21</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>838</v>
+        <v>23</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>839</v>
+        <v>16</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>837</v>
+        <v>17</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>18</v>
@@ -17295,343 +17268,343 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>831</v>
+        <v>20</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>836</v>
+        <v>21</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>838</v>
+        <v>23</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>837</v>
+        <v>16</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>833</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>834</v>
+        <v>10</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>833</v>
+        <v>23</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>792</v>
+        <v>806</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>792</v>
+        <v>806</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>792</v>
+        <v>806</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>792</v>
+        <v>806</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>792</v>
+        <v>801</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>833</v>
+        <v>19</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>10</v>
@@ -17639,119 +17612,119 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>834</v>
+        <v>16</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>831</v>
+        <v>25</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>837</v>
+        <v>23</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>831</v>
+        <v>10</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>23</v>
@@ -17759,7 +17732,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>16</v>
@@ -17767,7 +17740,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>17</v>
@@ -17775,23 +17748,23 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>831</v>
+        <v>23</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>16</v>
@@ -17799,159 +17772,159 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>838</v>
+        <v>17</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>811</v>
+        <v>562</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>811</v>
+        <v>562</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>837</v>
+        <v>20</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>810</v>
+        <v>562</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>810</v>
+        <v>562</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>810</v>
+        <v>562</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>562</v>
+        <v>818</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>562</v>
+        <v>818</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>834</v>
+        <v>25</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>562</v>
+        <v>820</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>562</v>
+        <v>820</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>562</v>
+        <v>817</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>837</v>
+        <v>16</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>18</v>
@@ -17959,63 +17932,63 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>834</v>
+        <v>18</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>838</v>
+        <v>16</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>834</v>
+        <v>21</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>16</v>
@@ -18023,167 +17996,167 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>838</v>
+        <v>25</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>834</v>
+        <v>16</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>834</v>
+        <v>10</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>838</v>
+        <v>16</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>834</v>
+        <v>25</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>16</v>
@@ -18191,153 +18164,49 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>838</v>
+        <v>18</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>834</v>
+        <v>22</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="B397" s="1" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="B398" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B399" s="1" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B400" s="1" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B401" s="1" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B402" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B403" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B404" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B405" s="1" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B406" s="1" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B407" s="1" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B408" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B409" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Default attachments functionality added
</commit_message>
<xml_diff>
--- a/server/database/seeds/seeds.xlsx
+++ b/server/database/seeds/seeds.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAACD89-891F-4DBB-94FF-E4358B76DE62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA677770-F6B9-4139-8080-318C3B708583}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40125" yWindow="705" windowWidth="25620" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guns" sheetId="1" r:id="rId1"/>
     <sheet name="Attachments" sheetId="3" r:id="rId2"/>
+    <sheet name="DefaultAttachments" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3357" uniqueCount="2202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3359" uniqueCount="2204">
   <si>
     <t>name</t>
   </si>
@@ -6627,6 +6628,12 @@
   </si>
   <si>
     <t>https://iili.io/HDHdue.png</t>
+  </si>
+  <si>
+    <t>gun_id</t>
+  </si>
+  <si>
+    <t>attachment_id</t>
   </si>
 </sst>
 </file>
@@ -6676,7 +6683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6688,11 +6695,107 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9999FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7446,7 +7549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7461,31 +7566,37 @@
     <col min="15" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -9446,146 +9557,146 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="C3:C65">
-    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="20" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="23" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="24" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="25" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="26" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="27" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="28" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="29" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="30" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="31" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="32" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="33" operator="equal">
       <formula>"Designated marksman rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
       <formula>"Shotgun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
       <formula>"Submachine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Assault carbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"Assault rifle"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D65">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>603</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"Designated marksman rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"Shotgun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"Submachine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"Assault carbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"Assault rifle"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="8" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="40" operator="equal">
       <formula>"Light machine gun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="45" operator="equal">
       <formula>"Pistol"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
       <formula>"Sniper rifle"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="52" operator="equal">
       <formula>"DMR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="53" operator="equal">
       <formula>"Shotgun"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="54" operator="equal">
       <formula>"SMG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="56" operator="equal">
       <formula>"Assault carbine"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="57" operator="equal">
       <formula>"Assault rifle"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9598,8 +9709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ED6926-697D-47E2-A2FD-3B0DE769BE34}">
   <dimension ref="A1:G1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="E210" sqref="E210"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9613,26 +9724,26 @@
     <col min="7" max="7" width="166.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2044</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>2045</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>2046</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>2047</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -29760,10 +29871,3866 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1015">
     <sortCondition ref="B2"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A946EE06-1CE7-4F34-A45B-74DFF0730608}">
+  <dimension ref="A1:B476"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="B65">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>8</v>
+      </c>
+      <c r="B66">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>10</v>
+      </c>
+      <c r="B74">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>11</v>
+      </c>
+      <c r="B75">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>11</v>
+      </c>
+      <c r="B78">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>11</v>
+      </c>
+      <c r="B79">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>11</v>
+      </c>
+      <c r="B80">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>11</v>
+      </c>
+      <c r="B81">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>11</v>
+      </c>
+      <c r="B82">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>12</v>
+      </c>
+      <c r="B83">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>12</v>
+      </c>
+      <c r="B84">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>12</v>
+      </c>
+      <c r="B85">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>12</v>
+      </c>
+      <c r="B86">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>12</v>
+      </c>
+      <c r="B87">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>12</v>
+      </c>
+      <c r="B88">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>12</v>
+      </c>
+      <c r="B89">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>12</v>
+      </c>
+      <c r="B90">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>13</v>
+      </c>
+      <c r="B91">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>13</v>
+      </c>
+      <c r="B92">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>13</v>
+      </c>
+      <c r="B93">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>13</v>
+      </c>
+      <c r="B94">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>13</v>
+      </c>
+      <c r="B95">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>13</v>
+      </c>
+      <c r="B96">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>13</v>
+      </c>
+      <c r="B97">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>13</v>
+      </c>
+      <c r="B98">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>14</v>
+      </c>
+      <c r="B99">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>14</v>
+      </c>
+      <c r="B100">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>14</v>
+      </c>
+      <c r="B101">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>14</v>
+      </c>
+      <c r="B102">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>14</v>
+      </c>
+      <c r="B103">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>14</v>
+      </c>
+      <c r="B104">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>14</v>
+      </c>
+      <c r="B105">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>14</v>
+      </c>
+      <c r="B106">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>15</v>
+      </c>
+      <c r="B107">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>15</v>
+      </c>
+      <c r="B108">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>15</v>
+      </c>
+      <c r="B109">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>15</v>
+      </c>
+      <c r="B110">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>15</v>
+      </c>
+      <c r="B111">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>15</v>
+      </c>
+      <c r="B112">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>15</v>
+      </c>
+      <c r="B113">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>15</v>
+      </c>
+      <c r="B114">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>16</v>
+      </c>
+      <c r="B115">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>16</v>
+      </c>
+      <c r="B116">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>16</v>
+      </c>
+      <c r="B117">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>16</v>
+      </c>
+      <c r="B118">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>16</v>
+      </c>
+      <c r="B119">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>16</v>
+      </c>
+      <c r="B120">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>16</v>
+      </c>
+      <c r="B121">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>16</v>
+      </c>
+      <c r="B122">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>17</v>
+      </c>
+      <c r="B123">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>17</v>
+      </c>
+      <c r="B124">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>17</v>
+      </c>
+      <c r="B125">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>17</v>
+      </c>
+      <c r="B126">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>17</v>
+      </c>
+      <c r="B127">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>17</v>
+      </c>
+      <c r="B128">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>18</v>
+      </c>
+      <c r="B129">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>18</v>
+      </c>
+      <c r="B130">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>18</v>
+      </c>
+      <c r="B131">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>18</v>
+      </c>
+      <c r="B132">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>18</v>
+      </c>
+      <c r="B133">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>18</v>
+      </c>
+      <c r="B134">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>19</v>
+      </c>
+      <c r="B135">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>19</v>
+      </c>
+      <c r="B136">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>19</v>
+      </c>
+      <c r="B137">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>19</v>
+      </c>
+      <c r="B138">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>19</v>
+      </c>
+      <c r="B139">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>19</v>
+      </c>
+      <c r="B140">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>20</v>
+      </c>
+      <c r="B141">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>20</v>
+      </c>
+      <c r="B142">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>20</v>
+      </c>
+      <c r="B143">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>20</v>
+      </c>
+      <c r="B144">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>20</v>
+      </c>
+      <c r="B145">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>20</v>
+      </c>
+      <c r="B146">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>20</v>
+      </c>
+      <c r="B147">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>21</v>
+      </c>
+      <c r="B148">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>21</v>
+      </c>
+      <c r="B149">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>21</v>
+      </c>
+      <c r="B150">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>21</v>
+      </c>
+      <c r="B151">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>21</v>
+      </c>
+      <c r="B152">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>21</v>
+      </c>
+      <c r="B153">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>21</v>
+      </c>
+      <c r="B154">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>22</v>
+      </c>
+      <c r="B155">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>22</v>
+      </c>
+      <c r="B156">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>22</v>
+      </c>
+      <c r="B157">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>22</v>
+      </c>
+      <c r="B158">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>22</v>
+      </c>
+      <c r="B159">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>22</v>
+      </c>
+      <c r="B160">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>22</v>
+      </c>
+      <c r="B161">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>22</v>
+      </c>
+      <c r="B162">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>22</v>
+      </c>
+      <c r="B163">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>22</v>
+      </c>
+      <c r="B164">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>22</v>
+      </c>
+      <c r="B165">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>23</v>
+      </c>
+      <c r="B166">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>23</v>
+      </c>
+      <c r="B167">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>23</v>
+      </c>
+      <c r="B168">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>23</v>
+      </c>
+      <c r="B169">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>23</v>
+      </c>
+      <c r="B170">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>23</v>
+      </c>
+      <c r="B171">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>23</v>
+      </c>
+      <c r="B172">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>23</v>
+      </c>
+      <c r="B173">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>24</v>
+      </c>
+      <c r="B174">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>24</v>
+      </c>
+      <c r="B175">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>24</v>
+      </c>
+      <c r="B176">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>24</v>
+      </c>
+      <c r="B177">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>24</v>
+      </c>
+      <c r="B178">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>25</v>
+      </c>
+      <c r="B179">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>25</v>
+      </c>
+      <c r="B180">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>25</v>
+      </c>
+      <c r="B181">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>25</v>
+      </c>
+      <c r="B182">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>25</v>
+      </c>
+      <c r="B183">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>26</v>
+      </c>
+      <c r="B184">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>26</v>
+      </c>
+      <c r="B185">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>26</v>
+      </c>
+      <c r="B186">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>26</v>
+      </c>
+      <c r="B187">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>26</v>
+      </c>
+      <c r="B188">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>26</v>
+      </c>
+      <c r="B189">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>27</v>
+      </c>
+      <c r="B190">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>27</v>
+      </c>
+      <c r="B191">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>27</v>
+      </c>
+      <c r="B192">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>27</v>
+      </c>
+      <c r="B193">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>27</v>
+      </c>
+      <c r="B194">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>28</v>
+      </c>
+      <c r="B195">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>28</v>
+      </c>
+      <c r="B196">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>28</v>
+      </c>
+      <c r="B197">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>28</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>28</v>
+      </c>
+      <c r="B199">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>28</v>
+      </c>
+      <c r="B200">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>28</v>
+      </c>
+      <c r="B201">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>28</v>
+      </c>
+      <c r="B202">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>28</v>
+      </c>
+      <c r="B203">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>28</v>
+      </c>
+      <c r="B204">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>29</v>
+      </c>
+      <c r="B205">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>29</v>
+      </c>
+      <c r="B206">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>29</v>
+      </c>
+      <c r="B207">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>29</v>
+      </c>
+      <c r="B208">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>29</v>
+      </c>
+      <c r="B209">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>30</v>
+      </c>
+      <c r="B210">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>30</v>
+      </c>
+      <c r="B211">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>30</v>
+      </c>
+      <c r="B212">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>30</v>
+      </c>
+      <c r="B213">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>30</v>
+      </c>
+      <c r="B214">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>31</v>
+      </c>
+      <c r="B215">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>31</v>
+      </c>
+      <c r="B216">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>31</v>
+      </c>
+      <c r="B217">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>31</v>
+      </c>
+      <c r="B218">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>31</v>
+      </c>
+      <c r="B219">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>31</v>
+      </c>
+      <c r="B220">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>31</v>
+      </c>
+      <c r="B221">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>31</v>
+      </c>
+      <c r="B222">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>31</v>
+      </c>
+      <c r="B223">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>31</v>
+      </c>
+      <c r="B224">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>31</v>
+      </c>
+      <c r="B225">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>32</v>
+      </c>
+      <c r="B226">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>32</v>
+      </c>
+      <c r="B227">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>32</v>
+      </c>
+      <c r="B228">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>32</v>
+      </c>
+      <c r="B229">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>32</v>
+      </c>
+      <c r="B230">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>32</v>
+      </c>
+      <c r="B231">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>32</v>
+      </c>
+      <c r="B232">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>33</v>
+      </c>
+      <c r="B233">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>33</v>
+      </c>
+      <c r="B234">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>33</v>
+      </c>
+      <c r="B235">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>33</v>
+      </c>
+      <c r="B236">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>33</v>
+      </c>
+      <c r="B237">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>33</v>
+      </c>
+      <c r="B238">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>34</v>
+      </c>
+      <c r="B239">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>34</v>
+      </c>
+      <c r="B240">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>34</v>
+      </c>
+      <c r="B241">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>34</v>
+      </c>
+      <c r="B242">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>34</v>
+      </c>
+      <c r="B243">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>35</v>
+      </c>
+      <c r="B244">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>35</v>
+      </c>
+      <c r="B245">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>35</v>
+      </c>
+      <c r="B246">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>35</v>
+      </c>
+      <c r="B247">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>35</v>
+      </c>
+      <c r="B248">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>36</v>
+      </c>
+      <c r="B249">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>36</v>
+      </c>
+      <c r="B250">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>36</v>
+      </c>
+      <c r="B251">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>36</v>
+      </c>
+      <c r="B252">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>36</v>
+      </c>
+      <c r="B253">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>36</v>
+      </c>
+      <c r="B254">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>36</v>
+      </c>
+      <c r="B255">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>37</v>
+      </c>
+      <c r="B256">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>37</v>
+      </c>
+      <c r="B257">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>37</v>
+      </c>
+      <c r="B258">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>37</v>
+      </c>
+      <c r="B259">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>37</v>
+      </c>
+      <c r="B260">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>37</v>
+      </c>
+      <c r="B261">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>37</v>
+      </c>
+      <c r="B262">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>38</v>
+      </c>
+      <c r="B263">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>38</v>
+      </c>
+      <c r="B264">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>38</v>
+      </c>
+      <c r="B265">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>38</v>
+      </c>
+      <c r="B266">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>38</v>
+      </c>
+      <c r="B267">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>38</v>
+      </c>
+      <c r="B268">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>38</v>
+      </c>
+      <c r="B269">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>39</v>
+      </c>
+      <c r="B270">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>39</v>
+      </c>
+      <c r="B271">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>39</v>
+      </c>
+      <c r="B272">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>39</v>
+      </c>
+      <c r="B273">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>39</v>
+      </c>
+      <c r="B274">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>39</v>
+      </c>
+      <c r="B275">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>39</v>
+      </c>
+      <c r="B276">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>39</v>
+      </c>
+      <c r="B277">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>39</v>
+      </c>
+      <c r="B278">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>39</v>
+      </c>
+      <c r="B279">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>39</v>
+      </c>
+      <c r="B280">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>39</v>
+      </c>
+      <c r="B281">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>40</v>
+      </c>
+      <c r="B282">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>40</v>
+      </c>
+      <c r="B283">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>40</v>
+      </c>
+      <c r="B284">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>40</v>
+      </c>
+      <c r="B285">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>40</v>
+      </c>
+      <c r="B286">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>40</v>
+      </c>
+      <c r="B287">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>40</v>
+      </c>
+      <c r="B288">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>40</v>
+      </c>
+      <c r="B289">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>40</v>
+      </c>
+      <c r="B290">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>40</v>
+      </c>
+      <c r="B291">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>40</v>
+      </c>
+      <c r="B292">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>40</v>
+      </c>
+      <c r="B293">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>40</v>
+      </c>
+      <c r="B294">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>41</v>
+      </c>
+      <c r="B295">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>41</v>
+      </c>
+      <c r="B296">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>41</v>
+      </c>
+      <c r="B297">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>41</v>
+      </c>
+      <c r="B298">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>41</v>
+      </c>
+      <c r="B299">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>42</v>
+      </c>
+      <c r="B300">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>42</v>
+      </c>
+      <c r="B301">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>42</v>
+      </c>
+      <c r="B302">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>42</v>
+      </c>
+      <c r="B303">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>42</v>
+      </c>
+      <c r="B304">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>43</v>
+      </c>
+      <c r="B305">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>43</v>
+      </c>
+      <c r="B306">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>43</v>
+      </c>
+      <c r="B307">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>43</v>
+      </c>
+      <c r="B308">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>43</v>
+      </c>
+      <c r="B309">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>44</v>
+      </c>
+      <c r="B310">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>44</v>
+      </c>
+      <c r="B311">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>44</v>
+      </c>
+      <c r="B312">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>44</v>
+      </c>
+      <c r="B313">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>45</v>
+      </c>
+      <c r="B314">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>45</v>
+      </c>
+      <c r="B315">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>45</v>
+      </c>
+      <c r="B316">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>45</v>
+      </c>
+      <c r="B317">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>46</v>
+      </c>
+      <c r="B318">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>46</v>
+      </c>
+      <c r="B319">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>46</v>
+      </c>
+      <c r="B320">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>46</v>
+      </c>
+      <c r="B321">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>46</v>
+      </c>
+      <c r="B322">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>46</v>
+      </c>
+      <c r="B323">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>46</v>
+      </c>
+      <c r="B324">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>46</v>
+      </c>
+      <c r="B325">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>46</v>
+      </c>
+      <c r="B326">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>46</v>
+      </c>
+      <c r="B327">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>46</v>
+      </c>
+      <c r="B328">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>46</v>
+      </c>
+      <c r="B329">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>46</v>
+      </c>
+      <c r="B330">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>47</v>
+      </c>
+      <c r="B331">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>47</v>
+      </c>
+      <c r="B332">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>47</v>
+      </c>
+      <c r="B333">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>47</v>
+      </c>
+      <c r="B334">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>47</v>
+      </c>
+      <c r="B335">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>47</v>
+      </c>
+      <c r="B336">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>48</v>
+      </c>
+      <c r="B337">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>48</v>
+      </c>
+      <c r="B338">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>48</v>
+      </c>
+      <c r="B339">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>49</v>
+      </c>
+      <c r="B340">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>50</v>
+      </c>
+      <c r="B341">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>51</v>
+      </c>
+      <c r="B342">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>51</v>
+      </c>
+      <c r="B343">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>52</v>
+      </c>
+      <c r="B344">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>52</v>
+      </c>
+      <c r="B345">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>53</v>
+      </c>
+      <c r="B346">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>53</v>
+      </c>
+      <c r="B347">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>53</v>
+      </c>
+      <c r="B348">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>53</v>
+      </c>
+      <c r="B349">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>54</v>
+      </c>
+      <c r="B350">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>54</v>
+      </c>
+      <c r="B351">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>54</v>
+      </c>
+      <c r="B352">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>55</v>
+      </c>
+      <c r="B353">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>55</v>
+      </c>
+      <c r="B354">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>55</v>
+      </c>
+      <c r="B355">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>55</v>
+      </c>
+      <c r="B356">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>56</v>
+      </c>
+      <c r="B357">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>56</v>
+      </c>
+      <c r="B358">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>56</v>
+      </c>
+      <c r="B359">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>56</v>
+      </c>
+      <c r="B360">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>56</v>
+      </c>
+      <c r="B361">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>56</v>
+      </c>
+      <c r="B362">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>56</v>
+      </c>
+      <c r="B363">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>56</v>
+      </c>
+      <c r="B364">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>57</v>
+      </c>
+      <c r="B365">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>57</v>
+      </c>
+      <c r="B366">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>57</v>
+      </c>
+      <c r="B367">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>57</v>
+      </c>
+      <c r="B368">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>57</v>
+      </c>
+      <c r="B369">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>57</v>
+      </c>
+      <c r="B370">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>57</v>
+      </c>
+      <c r="B371">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>58</v>
+      </c>
+      <c r="B372">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>58</v>
+      </c>
+      <c r="B373">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>58</v>
+      </c>
+      <c r="B374">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>58</v>
+      </c>
+      <c r="B375">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>58</v>
+      </c>
+      <c r="B376">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>58</v>
+      </c>
+      <c r="B377">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>58</v>
+      </c>
+      <c r="B378">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>58</v>
+      </c>
+      <c r="B379">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>59</v>
+      </c>
+      <c r="B380">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>59</v>
+      </c>
+      <c r="B381">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>59</v>
+      </c>
+      <c r="B382">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>59</v>
+      </c>
+      <c r="B383">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>59</v>
+      </c>
+      <c r="B384">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>59</v>
+      </c>
+      <c r="B385">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>59</v>
+      </c>
+      <c r="B386">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>59</v>
+      </c>
+      <c r="B387">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>59</v>
+      </c>
+      <c r="B388">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>59</v>
+      </c>
+      <c r="B389">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>59</v>
+      </c>
+      <c r="B390">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>59</v>
+      </c>
+      <c r="B391">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>59</v>
+      </c>
+      <c r="B392">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>60</v>
+      </c>
+      <c r="B393">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>60</v>
+      </c>
+      <c r="B394">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>60</v>
+      </c>
+      <c r="B395">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>60</v>
+      </c>
+      <c r="B396">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>60</v>
+      </c>
+      <c r="B397">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>60</v>
+      </c>
+      <c r="B398">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>61</v>
+      </c>
+      <c r="B399">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>61</v>
+      </c>
+      <c r="B400">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>61</v>
+      </c>
+      <c r="B401">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>62</v>
+      </c>
+      <c r="B402">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>62</v>
+      </c>
+      <c r="B403">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>62</v>
+      </c>
+      <c r="B404">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>63</v>
+      </c>
+      <c r="B405">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>63</v>
+      </c>
+      <c r="B406">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>63</v>
+      </c>
+      <c r="B407">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>63</v>
+      </c>
+      <c r="B408">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>63</v>
+      </c>
+      <c r="B409">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>64</v>
+      </c>
+      <c r="B410">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>64</v>
+      </c>
+      <c r="B411">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>64</v>
+      </c>
+      <c r="B412">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>64</v>
+      </c>
+      <c r="B413">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>64</v>
+      </c>
+      <c r="B414">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>64</v>
+      </c>
+      <c r="B415">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>64</v>
+      </c>
+      <c r="B416">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>65</v>
+      </c>
+      <c r="B417">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>65</v>
+      </c>
+      <c r="B418">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>65</v>
+      </c>
+      <c r="B419">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>65</v>
+      </c>
+      <c r="B420">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>66</v>
+      </c>
+      <c r="B421">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>66</v>
+      </c>
+      <c r="B422">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>66</v>
+      </c>
+      <c r="B423">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>66</v>
+      </c>
+      <c r="B424">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>66</v>
+      </c>
+      <c r="B425">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>66</v>
+      </c>
+      <c r="B426">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>66</v>
+      </c>
+      <c r="B427">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>66</v>
+      </c>
+      <c r="B428">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>67</v>
+      </c>
+      <c r="B429">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>67</v>
+      </c>
+      <c r="B430">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>67</v>
+      </c>
+      <c r="B431">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>67</v>
+      </c>
+      <c r="B432">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>67</v>
+      </c>
+      <c r="B433">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>68</v>
+      </c>
+      <c r="B434">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>68</v>
+      </c>
+      <c r="B435">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>68</v>
+      </c>
+      <c r="B436">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>68</v>
+      </c>
+      <c r="B437">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>68</v>
+      </c>
+      <c r="B438">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>68</v>
+      </c>
+      <c r="B439">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>68</v>
+      </c>
+      <c r="B440">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>68</v>
+      </c>
+      <c r="B441">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>68</v>
+      </c>
+      <c r="B442">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>68</v>
+      </c>
+      <c r="B443">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>68</v>
+      </c>
+      <c r="B444">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>69</v>
+      </c>
+      <c r="B445">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>69</v>
+      </c>
+      <c r="B446">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>69</v>
+      </c>
+      <c r="B447">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>70</v>
+      </c>
+      <c r="B448">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>70</v>
+      </c>
+      <c r="B449">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>70</v>
+      </c>
+      <c r="B450">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>71</v>
+      </c>
+      <c r="B451">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>71</v>
+      </c>
+      <c r="B452">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>71</v>
+      </c>
+      <c r="B453">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>72</v>
+      </c>
+      <c r="B454">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>72</v>
+      </c>
+      <c r="B455">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>72</v>
+      </c>
+      <c r="B456">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>72</v>
+      </c>
+      <c r="B457">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>72</v>
+      </c>
+      <c r="B458">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>72</v>
+      </c>
+      <c r="B459">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>72</v>
+      </c>
+      <c r="B460">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>72</v>
+      </c>
+      <c r="B461">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>74</v>
+      </c>
+      <c r="B462">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>74</v>
+      </c>
+      <c r="B463">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>74</v>
+      </c>
+      <c r="B464">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>74</v>
+      </c>
+      <c r="B465">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>74</v>
+      </c>
+      <c r="B466">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>74</v>
+      </c>
+      <c r="B467">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>74</v>
+      </c>
+      <c r="B468">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>74</v>
+      </c>
+      <c r="B469">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>73</v>
+      </c>
+      <c r="B470">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>73</v>
+      </c>
+      <c r="B471">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>73</v>
+      </c>
+      <c r="B472">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>73</v>
+      </c>
+      <c r="B473">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>73</v>
+      </c>
+      <c r="B474">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>75</v>
+      </c>
+      <c r="B475">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>75</v>
+      </c>
+      <c r="B476">
+        <v>696</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"Light machine gun"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"Pistol"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Sniper rifle"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"DMR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Shotgun"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"SMG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+      <formula>"Assault carbine"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+      <formula>"Assault rifle"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>